<commit_message>
Conclusão programa de inclusão
</commit_message>
<xml_diff>
--- a/DB2/MAPDB2C.xlsx
+++ b/DB2/MAPDB2C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dynamic\Mainframe\DB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0072720-8D85-43A8-977E-DD34BE7C709E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC449740-FF9E-4C30-ADF8-DC8A1CA613DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19980" windowHeight="14865" xr2:uid="{EA64248A-43C7-4D0B-8895-3E5C2BC5B090}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19980" windowHeight="15315" xr2:uid="{EA64248A-43C7-4D0B-8895-3E5C2BC5B090}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="40">
   <si>
     <t>I</t>
   </si>
@@ -264,15 +264,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -610,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30331CBE-3728-4B64-BBB7-33697854CB59}">
-  <dimension ref="A1:CF32"/>
+  <dimension ref="A1:CF31"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="55" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="BP3" sqref="BP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.140625" defaultRowHeight="14.25"/>
@@ -622,357 +619,357 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:84" ht="16.5">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3" t="s">
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3" t="s">
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3" t="s">
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3"/>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
-      <c r="BI1" s="3"/>
-      <c r="BJ1" s="3"/>
-      <c r="BK1" s="3" t="s">
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+      <c r="BD1" s="9"/>
+      <c r="BE1" s="9"/>
+      <c r="BF1" s="9"/>
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="9"/>
+      <c r="BK1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3"/>
-      <c r="BO1" s="3"/>
-      <c r="BP1" s="3"/>
-      <c r="BQ1" s="3"/>
-      <c r="BR1" s="3"/>
-      <c r="BS1" s="3"/>
-      <c r="BT1" s="3"/>
-      <c r="BU1" s="3" t="s">
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="9"/>
+      <c r="BU1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BV1" s="3"/>
-      <c r="BW1" s="3"/>
-      <c r="BX1" s="3"/>
-      <c r="BY1" s="3"/>
-      <c r="BZ1" s="3"/>
-      <c r="CA1" s="3"/>
-      <c r="CB1" s="3"/>
-      <c r="CC1" s="3"/>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3"/>
-      <c r="CF1" s="3"/>
+      <c r="BV1" s="9"/>
+      <c r="BW1" s="9"/>
+      <c r="BX1" s="9"/>
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9"/>
+      <c r="CA1" s="9"/>
+      <c r="CB1" s="9"/>
+      <c r="CC1" s="9"/>
+      <c r="CD1" s="9"/>
+      <c r="CE1" s="9"/>
+      <c r="CF1" s="9"/>
     </row>
     <row r="2" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W2" s="3" t="s">
+      <c r="V2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AF2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AP2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AP2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AS2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AT2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AU2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AV2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AW2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AX2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AY2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AZ2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BA2" s="3" t="s">
+      <c r="AZ2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BB2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BC2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BD2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BE2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BF2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BG2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BH2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BI2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="BJ2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BK2" s="3" t="s">
+      <c r="BJ2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="BL2" s="3" t="s">
+      <c r="BL2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="BM2" s="3" t="s">
+      <c r="BM2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="BN2" s="3" t="s">
+      <c r="BN2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="BO2" s="3" t="s">
+      <c r="BO2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BP2" s="3" t="s">
+      <c r="BP2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="BS2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BT2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BU2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BV2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="BW2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="BX2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BQ2" s="3" t="s">
+      <c r="BZ2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="CA2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BR2" s="3" t="s">
+      <c r="CB2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BS2" s="3" t="s">
+      <c r="CC2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="BT2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BU2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="BV2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="BW2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="BX2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="BY2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BZ2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="CA2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="CB2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="CC2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="CD2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="CE2" s="3"/>
-      <c r="CF2" s="3"/>
+      <c r="CD2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE2" s="9"/>
+      <c r="CF2" s="9"/>
     </row>
     <row r="3" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1052,245 +1049,245 @@
       <c r="CB3" s="2"/>
       <c r="CC3" s="2"/>
       <c r="CD3" s="2"/>
-      <c r="CE3" s="3" t="s">
+      <c r="CE3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="CF3" s="3"/>
+      <c r="CF3" s="9"/>
     </row>
     <row r="4" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="4" t="s">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="4" t="s">
+      <c r="M4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R4" s="4" t="s">
+      <c r="P4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4" t="s">
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z4" s="4" t="s">
+      <c r="Z4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AA4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AB4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AC4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AD4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AE4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AF4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AG4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AH4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AI4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AK4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AL4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AM4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AN4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AO4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AP4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AR4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AS4" s="4" t="s">
+      <c r="AS4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AT4" s="4" t="s">
+      <c r="AT4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AU4" s="4" t="s">
+      <c r="AU4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AV4" s="4" t="s">
+      <c r="AV4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AW4" s="4" t="s">
+      <c r="AW4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AX4" s="4" t="s">
+      <c r="AX4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="4" t="s">
+      <c r="AY4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AZ4" s="4" t="s">
+      <c r="AZ4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="BA4" s="4" t="s">
+      <c r="BA4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BB4" s="4" t="s">
+      <c r="BB4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BC4" s="4" t="s">
+      <c r="BC4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="BD4" s="4" t="s">
+      <c r="BD4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BE4" s="4" t="s">
+      <c r="BE4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="BF4" s="4" t="s">
+      <c r="BF4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BG4" s="4" t="s">
+      <c r="BG4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="BH4" s="4" t="s">
+      <c r="BH4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="BI4" s="4" t="s">
+      <c r="BI4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="BJ4" s="4" t="s">
+      <c r="BJ4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="BK4" s="4" t="s">
+      <c r="BK4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BL4" s="4"/>
-      <c r="BM4" s="4"/>
-      <c r="BN4" s="4"/>
-      <c r="BO4" s="4" t="s">
+      <c r="BL4" s="3"/>
+      <c r="BM4" s="3"/>
+      <c r="BN4" s="3"/>
+      <c r="BO4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BP4" s="4" t="s">
+      <c r="BP4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BQ4" s="4" t="s">
+      <c r="BQ4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BR4" s="4"/>
-      <c r="BS4" s="4" t="s">
+      <c r="BR4" s="3"/>
+      <c r="BS4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="BT4" s="4" t="s">
+      <c r="BT4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BU4" s="4" t="s">
+      <c r="BU4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BV4" s="4" t="s">
+      <c r="BV4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="BW4" s="4" t="s">
+      <c r="BW4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BX4" s="4" t="s">
+      <c r="BX4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BY4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="BZ4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="CA4" s="4" t="s">
+      <c r="BY4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="CB4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="CC4" s="4" t="s">
+      <c r="CB4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="CD4" s="2"/>
-      <c r="CE4" s="3" t="s">
+      <c r="CE4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="CF4" s="3"/>
+      <c r="CF4" s="9"/>
     </row>
     <row r="5" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1370,97 +1367,97 @@
       <c r="CB5" s="2"/>
       <c r="CC5" s="2"/>
       <c r="CD5" s="2"/>
-      <c r="CE5" s="3" t="s">
+      <c r="CE5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="CF5" s="3"/>
+      <c r="CF5" s="9"/>
     </row>
     <row r="6" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="5" t="s">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AG6" s="5" t="s">
+      <c r="AG6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH6" s="5" t="s">
+      <c r="AH6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AI6" s="5" t="s">
+      <c r="AI6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AJ6" s="5" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AK6" s="5" t="s">
+      <c r="AK6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AL6" s="5" t="s">
+      <c r="AL6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AM6" s="5" t="s">
+      <c r="AM6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="5" t="s">
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AP6" s="5" t="s">
+      <c r="AP6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AQ6" s="5"/>
+      <c r="AQ6" s="4"/>
       <c r="AR6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1488,73 +1485,73 @@
       <c r="AZ6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="BA6" s="4"/>
-      <c r="BB6" s="4"/>
-      <c r="BC6" s="4"/>
-      <c r="BD6" s="4"/>
-      <c r="BE6" s="4"/>
-      <c r="BF6" s="4"/>
-      <c r="BG6" s="4"/>
-      <c r="BH6" s="4"/>
-      <c r="BI6" s="4"/>
-      <c r="BJ6" s="4"/>
-      <c r="BK6" s="4"/>
-      <c r="BL6" s="4"/>
-      <c r="BM6" s="4"/>
-      <c r="BN6" s="4"/>
-      <c r="BO6" s="4"/>
-      <c r="BP6" s="4" t="s">
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
+      <c r="BI6" s="3"/>
+      <c r="BJ6" s="3"/>
+      <c r="BK6" s="3"/>
+      <c r="BL6" s="3"/>
+      <c r="BM6" s="3"/>
+      <c r="BN6" s="3"/>
+      <c r="BO6" s="3"/>
+      <c r="BP6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BQ6" s="4" t="s">
+      <c r="BQ6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BR6" s="4"/>
-      <c r="BS6" s="4" t="s">
+      <c r="BR6" s="3"/>
+      <c r="BS6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="BT6" s="4" t="s">
+      <c r="BT6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="BU6" s="4" t="s">
+      <c r="BU6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BV6" s="4" t="s">
+      <c r="BV6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="BW6" s="4" t="s">
+      <c r="BW6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="BX6" s="4" t="s">
+      <c r="BX6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BY6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="BZ6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="CA6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="CB6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="CC6" s="4" t="s">
+      <c r="BY6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="BZ6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="CA6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="CB6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="CC6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="CD6" s="2"/>
-      <c r="CE6" s="3" t="s">
+      <c r="CE6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="CF6" s="3"/>
+      <c r="CF6" s="9"/>
     </row>
     <row r="7" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1634,17 +1631,17 @@
       <c r="CB7" s="2"/>
       <c r="CC7" s="2"/>
       <c r="CD7" s="2"/>
-      <c r="CE7" s="3" t="s">
+      <c r="CE7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CF7" s="3"/>
+      <c r="CF7" s="9"/>
     </row>
     <row r="8" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1724,17 +1721,17 @@
       <c r="CB8" s="2"/>
       <c r="CC8" s="2"/>
       <c r="CD8" s="2"/>
-      <c r="CE8" s="3" t="s">
+      <c r="CE8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="CF8" s="3"/>
+      <c r="CF8" s="9"/>
     </row>
     <row r="9" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2"/>
@@ -1816,47 +1813,47 @@
       <c r="CB9" s="2"/>
       <c r="CC9" s="2"/>
       <c r="CD9" s="2"/>
-      <c r="CE9" s="3" t="s">
+      <c r="CE9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="CF9" s="3"/>
+      <c r="CF9" s="9"/>
     </row>
     <row r="10" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -1940,17 +1937,17 @@
       <c r="CB10" s="2"/>
       <c r="CC10" s="2"/>
       <c r="CD10" s="2"/>
-      <c r="CE10" s="3" t="s">
+      <c r="CE10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CF10" s="3"/>
+      <c r="CF10" s="9"/>
     </row>
     <row r="11" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="2"/>
@@ -2034,19 +2031,19 @@
       <c r="CB11" s="2"/>
       <c r="CC11" s="2"/>
       <c r="CD11" s="2"/>
-      <c r="CE11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="CF11" s="3"/>
+      <c r="CE11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF11" s="9"/>
     </row>
     <row r="12" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2"/>
@@ -2128,49 +2125,49 @@
       <c r="CB12" s="2"/>
       <c r="CC12" s="2"/>
       <c r="CD12" s="2"/>
-      <c r="CE12" s="3" t="s">
+      <c r="CE12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="CF12" s="3" t="s">
+      <c r="CF12" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N13" s="2"/>
@@ -2302,17 +2299,17 @@
       <c r="CB13" s="2"/>
       <c r="CC13" s="2"/>
       <c r="CD13" s="2"/>
-      <c r="CE13" s="3" t="s">
+      <c r="CE13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="CF13" s="3"/>
+      <c r="CF13" s="9"/>
     </row>
     <row r="14" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2"/>
@@ -2394,47 +2391,47 @@
       <c r="CB14" s="2"/>
       <c r="CC14" s="2"/>
       <c r="CD14" s="2"/>
-      <c r="CE14" s="3" t="s">
+      <c r="CE14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="CF14" s="3"/>
+      <c r="CF14" s="9"/>
     </row>
     <row r="15" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N15" s="2"/>
@@ -2513,34 +2510,34 @@
       <c r="AU15" s="2"/>
       <c r="AV15" s="2"/>
       <c r="AW15" s="2"/>
-      <c r="AX15" s="5" t="s">
+      <c r="AX15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AY15" s="5" t="s">
+      <c r="AY15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AZ15" s="5" t="s">
+      <c r="AZ15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BA15" s="5" t="s">
+      <c r="BA15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="BB15" s="5" t="s">
+      <c r="BB15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="BC15" s="5" t="s">
+      <c r="BC15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BD15" s="5" t="s">
+      <c r="BD15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BE15" s="5" t="s">
+      <c r="BE15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BF15" s="5" t="s">
+      <c r="BF15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BG15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="BH15" s="2"/>
@@ -2596,30 +2593,30 @@
       <c r="CB15" s="2"/>
       <c r="CC15" s="2"/>
       <c r="CD15" s="2"/>
-      <c r="CE15" s="3" t="s">
+      <c r="CE15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="CF15" s="3"/>
+      <c r="CF15" s="9"/>
     </row>
     <row r="16" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -2656,16 +2653,16 @@
       <c r="AV16" s="2"/>
       <c r="AW16" s="2"/>
       <c r="AX16" s="2"/>
-      <c r="AY16" s="5"/>
-      <c r="AZ16" s="5"/>
-      <c r="BA16" s="5"/>
-      <c r="BB16" s="5"/>
-      <c r="BC16" s="5"/>
-      <c r="BD16" s="5"/>
-      <c r="BE16" s="5"/>
-      <c r="BF16" s="5"/>
-      <c r="BG16" s="5"/>
-      <c r="BH16" s="5"/>
+      <c r="AY16" s="4"/>
+      <c r="AZ16" s="4"/>
+      <c r="BA16" s="4"/>
+      <c r="BB16" s="4"/>
+      <c r="BC16" s="4"/>
+      <c r="BD16" s="4"/>
+      <c r="BE16" s="4"/>
+      <c r="BF16" s="4"/>
+      <c r="BG16" s="4"/>
+      <c r="BH16" s="4"/>
       <c r="BI16" s="2"/>
       <c r="BJ16" s="2"/>
       <c r="BK16" s="2"/>
@@ -2688,47 +2685,47 @@
       <c r="CB16" s="2"/>
       <c r="CC16" s="2"/>
       <c r="CD16" s="2"/>
-      <c r="CE16" s="3" t="s">
+      <c r="CE16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="CF16" s="3"/>
+      <c r="CF16" s="9"/>
     </row>
     <row r="17" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N17" s="2"/>
@@ -2827,34 +2824,34 @@
       <c r="AU17" s="2"/>
       <c r="AV17" s="2"/>
       <c r="AW17" s="2"/>
-      <c r="AX17" s="5" t="s">
+      <c r="AX17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AY17" s="5" t="s">
+      <c r="AY17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AZ17" s="5" t="s">
+      <c r="AZ17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BA17" s="5" t="s">
+      <c r="BA17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BB17" s="5" t="s">
+      <c r="BB17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BC17" s="5" t="s">
+      <c r="BC17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="BD17" s="5" t="s">
+      <c r="BD17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BE17" s="5" t="s">
+      <c r="BE17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BF17" s="5" t="s">
+      <c r="BF17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BG17" s="5" t="s">
+      <c r="BG17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="BH17" s="2"/>
@@ -2920,30 +2917,30 @@
       </c>
       <c r="CC17" s="2"/>
       <c r="CD17" s="2"/>
-      <c r="CE17" s="3" t="s">
+      <c r="CE17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CF17" s="3"/>
+      <c r="CF17" s="9"/>
     </row>
     <row r="18" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -2980,16 +2977,16 @@
       <c r="AV18" s="2"/>
       <c r="AW18" s="2"/>
       <c r="AX18" s="2"/>
-      <c r="AY18" s="5"/>
-      <c r="AZ18" s="5"/>
-      <c r="BA18" s="5"/>
-      <c r="BB18" s="5"/>
-      <c r="BC18" s="5"/>
-      <c r="BD18" s="5"/>
-      <c r="BE18" s="5"/>
-      <c r="BF18" s="5"/>
-      <c r="BG18" s="5"/>
-      <c r="BH18" s="5"/>
+      <c r="AY18" s="4"/>
+      <c r="AZ18" s="4"/>
+      <c r="BA18" s="4"/>
+      <c r="BB18" s="4"/>
+      <c r="BC18" s="4"/>
+      <c r="BD18" s="4"/>
+      <c r="BE18" s="4"/>
+      <c r="BF18" s="4"/>
+      <c r="BG18" s="4"/>
+      <c r="BH18" s="4"/>
       <c r="BI18" s="2"/>
       <c r="BJ18" s="2"/>
       <c r="BK18" s="2"/>
@@ -3012,47 +3009,47 @@
       <c r="CB18" s="2"/>
       <c r="CC18" s="2"/>
       <c r="CD18" s="2"/>
-      <c r="CE18" s="3" t="s">
+      <c r="CE18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="CF18" s="3"/>
+      <c r="CF18" s="9"/>
     </row>
     <row r="19" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N19" s="2"/>
@@ -3141,34 +3138,34 @@
       <c r="AU19" s="2"/>
       <c r="AV19" s="2"/>
       <c r="AW19" s="2"/>
-      <c r="AX19" s="5" t="s">
+      <c r="AX19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AY19" s="5" t="s">
+      <c r="AY19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AZ19" s="5" t="s">
+      <c r="AZ19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="BA19" s="5" t="s">
+      <c r="BA19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="BB19" s="5" t="s">
+      <c r="BB19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="BC19" s="5" t="s">
+      <c r="BC19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="BD19" s="5" t="s">
+      <c r="BD19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BE19" s="5" t="s">
+      <c r="BE19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BF19" s="5" t="s">
+      <c r="BF19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BG19" s="5" t="s">
+      <c r="BG19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="BH19" s="2"/>
@@ -3198,30 +3195,30 @@
       <c r="CB19" s="2"/>
       <c r="CC19" s="2"/>
       <c r="CD19" s="2"/>
-      <c r="CE19" s="3" t="s">
+      <c r="CE19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="CF19" s="3"/>
+      <c r="CF19" s="9"/>
     </row>
     <row r="20" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
@@ -3258,16 +3255,16 @@
       <c r="AV20" s="2"/>
       <c r="AW20" s="2"/>
       <c r="AX20" s="2"/>
-      <c r="AY20" s="5"/>
-      <c r="AZ20" s="5"/>
-      <c r="BA20" s="5"/>
-      <c r="BB20" s="5"/>
-      <c r="BC20" s="5"/>
-      <c r="BD20" s="5"/>
-      <c r="BE20" s="5"/>
-      <c r="BF20" s="5"/>
-      <c r="BG20" s="5"/>
-      <c r="BH20" s="5"/>
+      <c r="AY20" s="4"/>
+      <c r="AZ20" s="4"/>
+      <c r="BA20" s="4"/>
+      <c r="BB20" s="4"/>
+      <c r="BC20" s="4"/>
+      <c r="BD20" s="4"/>
+      <c r="BE20" s="4"/>
+      <c r="BF20" s="4"/>
+      <c r="BG20" s="4"/>
+      <c r="BH20" s="4"/>
       <c r="BI20" s="2"/>
       <c r="BJ20" s="2"/>
       <c r="BK20" s="2"/>
@@ -3290,45 +3287,45 @@
       <c r="CB20" s="2"/>
       <c r="CC20" s="2"/>
       <c r="CD20" s="2"/>
-      <c r="CE20" s="3" t="s">
+      <c r="CE20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CF20" s="3"/>
+      <c r="CF20" s="9"/>
     </row>
     <row r="21" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="M21" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N21" s="2"/>
@@ -3427,34 +3424,34 @@
       <c r="AU21" s="2"/>
       <c r="AV21" s="2"/>
       <c r="AW21" s="2"/>
-      <c r="AX21" s="5" t="s">
+      <c r="AX21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AY21" s="5" t="s">
+      <c r="AY21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AZ21" s="5" t="s">
+      <c r="AZ21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="BA21" s="5" t="s">
+      <c r="BA21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="BB21" s="5" t="s">
+      <c r="BB21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="BC21" s="5" t="s">
+      <c r="BC21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="BD21" s="5" t="s">
+      <c r="BD21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BE21" s="5" t="s">
+      <c r="BE21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="BF21" s="5" t="s">
+      <c r="BF21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BG21" s="5" t="s">
+      <c r="BG21" s="4" t="s">
         <v>16</v>
       </c>
       <c r="BH21" s="2"/>
@@ -3504,19 +3501,19 @@
       <c r="CB21" s="2"/>
       <c r="CC21" s="2"/>
       <c r="CD21" s="2"/>
-      <c r="CE21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="CF21" s="3"/>
+      <c r="CE21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF21" s="9"/>
     </row>
     <row r="22" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -3596,19 +3593,19 @@
       <c r="CB22" s="2"/>
       <c r="CC22" s="2"/>
       <c r="CD22" s="2"/>
-      <c r="CE22" s="3" t="s">
+      <c r="CE22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="CF22" s="3" t="s">
+      <c r="CF22" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -3688,17 +3685,17 @@
       <c r="CB23" s="2"/>
       <c r="CC23" s="2"/>
       <c r="CD23" s="2"/>
-      <c r="CE23" s="3" t="s">
+      <c r="CE23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="CF23" s="3"/>
+      <c r="CF23" s="9"/>
     </row>
     <row r="24" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -3778,249 +3775,249 @@
       <c r="CB24" s="2"/>
       <c r="CC24" s="2"/>
       <c r="CD24" s="2"/>
-      <c r="CE24" s="3" t="s">
+      <c r="CE24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="CF24" s="3"/>
+      <c r="CF24" s="9"/>
     </row>
     <row r="25" spans="1:84" ht="15.95" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4" t="s">
+      <c r="L25" s="3"/>
+      <c r="M25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="N25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="R25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="T25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AS25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AU25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AV25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AY25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AZ25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BA25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BB25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BC25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BD25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BE25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BF25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BG25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BH25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BI25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BJ25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BK25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BL25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BM25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BN25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BO25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BP25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BQ25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BR25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BS25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BT25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BU25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BV25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BW25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BX25" s="6"/>
-      <c r="BY25" s="6"/>
-      <c r="BZ25" s="6"/>
-      <c r="CA25" s="6"/>
-      <c r="CB25" s="6"/>
-      <c r="CC25" s="6" t="s">
+      <c r="O25" s="5"/>
+      <c r="P25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AV25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AZ25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BC25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BE25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BF25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BG25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BH25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BI25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BJ25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BK25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BL25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BM25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BN25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BO25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BP25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BQ25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BR25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BS25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BT25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BU25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BV25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BW25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BX25" s="5"/>
+      <c r="BY25" s="5"/>
+      <c r="BZ25" s="5"/>
+      <c r="CA25" s="5"/>
+      <c r="CB25" s="5"/>
+      <c r="CC25" s="5" t="s">
         <v>31</v>
       </c>
       <c r="CD25" s="2"/>
-      <c r="CE25" s="3" t="s">
+      <c r="CE25" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="CF25" s="3"/>
+      <c r="CF25" s="9"/>
     </row>
     <row r="26" spans="1:84" ht="16.5">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -4033,949 +4030,897 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
-      <c r="AE26" s="6"/>
-      <c r="AF26" s="6"/>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
-      <c r="AI26" s="6"/>
-      <c r="AJ26" s="6"/>
-      <c r="AK26" s="6"/>
-      <c r="AL26" s="6"/>
-      <c r="AM26" s="6"/>
-      <c r="AN26" s="6"/>
-      <c r="AO26" s="6"/>
-      <c r="AP26" s="6"/>
-      <c r="AQ26" s="6"/>
-      <c r="AR26" s="6"/>
-      <c r="AS26" s="6"/>
-      <c r="AT26" s="6"/>
-      <c r="AU26" s="6"/>
-      <c r="AV26" s="6"/>
-      <c r="AW26" s="6"/>
-      <c r="AX26" s="6"/>
-      <c r="AY26" s="6"/>
-      <c r="AZ26" s="6"/>
-      <c r="BA26" s="6"/>
-      <c r="BB26" s="6"/>
-      <c r="BC26" s="6"/>
-      <c r="BD26" s="6"/>
-      <c r="BE26" s="6"/>
-      <c r="BF26" s="6"/>
-      <c r="BG26" s="6"/>
-      <c r="BH26" s="6"/>
-      <c r="BI26" s="6"/>
-      <c r="BJ26" s="6"/>
-      <c r="BK26" s="6"/>
-      <c r="BL26" s="6"/>
-      <c r="BM26" s="6"/>
-      <c r="BN26" s="6"/>
-      <c r="BO26" s="6"/>
-      <c r="BP26" s="6"/>
-      <c r="BQ26" s="6"/>
-      <c r="BR26" s="6"/>
-      <c r="BS26" s="6"/>
-      <c r="BT26" s="6"/>
-      <c r="BU26" s="6"/>
-      <c r="BV26" s="6"/>
-      <c r="BW26" s="6"/>
-      <c r="BX26" s="6"/>
-      <c r="BY26" s="6"/>
-      <c r="BZ26" s="6"/>
-      <c r="CA26" s="6"/>
-      <c r="CB26" s="6"/>
-      <c r="CC26" s="6"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+      <c r="AQ26" s="5"/>
+      <c r="AR26" s="5"/>
+      <c r="AS26" s="5"/>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5"/>
+      <c r="AV26" s="5"/>
+      <c r="AW26" s="5"/>
+      <c r="AX26" s="5"/>
+      <c r="AY26" s="5"/>
+      <c r="AZ26" s="5"/>
+      <c r="BA26" s="5"/>
+      <c r="BB26" s="5"/>
+      <c r="BC26" s="5"/>
+      <c r="BD26" s="5"/>
+      <c r="BE26" s="5"/>
+      <c r="BF26" s="5"/>
+      <c r="BG26" s="5"/>
+      <c r="BH26" s="5"/>
+      <c r="BI26" s="5"/>
+      <c r="BJ26" s="5"/>
+      <c r="BK26" s="5"/>
+      <c r="BL26" s="5"/>
+      <c r="BM26" s="5"/>
+      <c r="BN26" s="5"/>
+      <c r="BO26" s="5"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5"/>
+      <c r="BR26" s="5"/>
+      <c r="BS26" s="5"/>
+      <c r="BT26" s="5"/>
+      <c r="BU26" s="5"/>
+      <c r="BV26" s="5"/>
+      <c r="BW26" s="5"/>
+      <c r="BX26" s="5"/>
+      <c r="BY26" s="5"/>
+      <c r="BZ26" s="5"/>
+      <c r="CA26" s="5"/>
+      <c r="CB26" s="5"/>
+      <c r="CC26" s="5"/>
       <c r="CD26" s="2"/>
-      <c r="CE26" s="3" t="s">
+      <c r="CE26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="CF26" s="3"/>
+      <c r="CF26" s="9"/>
     </row>
     <row r="27" spans="1:84" ht="16.5">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M27" s="3" t="s">
+      <c r="L27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="N27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="O27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="P27" s="3" t="s">
+      <c r="P27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Q27" s="3" t="s">
+      <c r="Q27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="R27" s="3" t="s">
+      <c r="R27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="S27" s="3" t="s">
+      <c r="S27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="T27" s="3" t="s">
+      <c r="T27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U27" s="3" t="s">
+      <c r="U27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W27" s="3" t="s">
+      <c r="V27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="W27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X27" s="3" t="s">
+      <c r="X27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Y27" s="3" t="s">
+      <c r="Y27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Z27" s="3" t="s">
+      <c r="Z27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AA27" s="3" t="s">
+      <c r="AA27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AB27" s="3" t="s">
+      <c r="AB27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AC27" s="3" t="s">
+      <c r="AC27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AD27" s="3" t="s">
+      <c r="AD27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AE27" s="3" t="s">
+      <c r="AE27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AF27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG27" s="3" t="s">
+      <c r="AF27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AH27" s="3" t="s">
+      <c r="AH27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AI27" s="3" t="s">
+      <c r="AI27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AJ27" s="3" t="s">
+      <c r="AJ27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AK27" s="3" t="s">
+      <c r="AK27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AL27" s="3" t="s">
+      <c r="AL27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AM27" s="3" t="s">
+      <c r="AM27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AN27" s="3" t="s">
+      <c r="AN27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AO27" s="3" t="s">
+      <c r="AO27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AP27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ27" s="3" t="s">
+      <c r="AP27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AR27" s="3" t="s">
+      <c r="AR27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AS27" s="3" t="s">
+      <c r="AS27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AT27" s="3" t="s">
+      <c r="AT27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AU27" s="3" t="s">
+      <c r="AU27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AV27" s="3" t="s">
+      <c r="AV27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AW27" s="3" t="s">
+      <c r="AW27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AX27" s="3" t="s">
+      <c r="AX27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AY27" s="3" t="s">
+      <c r="AY27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AZ27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BA27" s="3" t="s">
+      <c r="AZ27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="BB27" s="3" t="s">
+      <c r="BB27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="BC27" s="3" t="s">
+      <c r="BC27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="BD27" s="3" t="s">
+      <c r="BD27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="BE27" s="3" t="s">
+      <c r="BE27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BF27" s="3" t="s">
+      <c r="BF27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BG27" s="3" t="s">
+      <c r="BG27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BH27" s="3" t="s">
+      <c r="BH27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BI27" s="3" t="s">
+      <c r="BI27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="BJ27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BK27" s="3" t="s">
+      <c r="BJ27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="BL27" s="3" t="s">
+      <c r="BL27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="BM27" s="3" t="s">
+      <c r="BM27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="BN27" s="3" t="s">
+      <c r="BN27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="BO27" s="3" t="s">
+      <c r="BO27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BP27" s="3" t="s">
+      <c r="BP27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BQ27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="BS27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BT27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BU27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BV27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="BW27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="BX27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BQ27" s="3" t="s">
+      <c r="BZ27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="CA27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BR27" s="3" t="s">
+      <c r="CB27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BS27" s="3" t="s">
+      <c r="CC27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="BT27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BU27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="BV27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="BW27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="BX27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="BY27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BZ27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="CA27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="CB27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="CC27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="CD27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="CE27" s="3"/>
-      <c r="CF27" s="3"/>
+      <c r="CD27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE27" s="9"/>
+      <c r="CF27" s="9"/>
     </row>
     <row r="28" spans="1:84" ht="16.5">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3" t="s">
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AA28" s="3"/>
-      <c r="AB28" s="3"/>
-      <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
-      <c r="AF28" s="3"/>
-      <c r="AG28" s="3" t="s">
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AH28" s="3"/>
-      <c r="AI28" s="3"/>
-      <c r="AJ28" s="3"/>
-      <c r="AK28" s="3"/>
-      <c r="AL28" s="3"/>
-      <c r="AM28" s="3"/>
-      <c r="AN28" s="3"/>
-      <c r="AO28" s="3"/>
-      <c r="AP28" s="3"/>
-      <c r="AQ28" s="3" t="s">
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="9"/>
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="9"/>
+      <c r="AN28" s="9"/>
+      <c r="AO28" s="9"/>
+      <c r="AP28" s="9"/>
+      <c r="AQ28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AR28" s="3"/>
-      <c r="AS28" s="3"/>
-      <c r="AT28" s="3"/>
-      <c r="AU28" s="3"/>
-      <c r="AV28" s="3"/>
-      <c r="AW28" s="3"/>
-      <c r="AX28" s="3"/>
-      <c r="AY28" s="3"/>
-      <c r="AZ28" s="3"/>
-      <c r="BA28" s="3" t="s">
+      <c r="AR28" s="9"/>
+      <c r="AS28" s="9"/>
+      <c r="AT28" s="9"/>
+      <c r="AU28" s="9"/>
+      <c r="AV28" s="9"/>
+      <c r="AW28" s="9"/>
+      <c r="AX28" s="9"/>
+      <c r="AY28" s="9"/>
+      <c r="AZ28" s="9"/>
+      <c r="BA28" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BB28" s="3"/>
-      <c r="BC28" s="3"/>
-      <c r="BD28" s="3"/>
-      <c r="BE28" s="3"/>
-      <c r="BF28" s="3"/>
-      <c r="BG28" s="3"/>
-      <c r="BH28" s="3"/>
-      <c r="BI28" s="3"/>
-      <c r="BJ28" s="3"/>
-      <c r="BK28" s="3" t="s">
+      <c r="BB28" s="9"/>
+      <c r="BC28" s="9"/>
+      <c r="BD28" s="9"/>
+      <c r="BE28" s="9"/>
+      <c r="BF28" s="9"/>
+      <c r="BG28" s="9"/>
+      <c r="BH28" s="9"/>
+      <c r="BI28" s="9"/>
+      <c r="BJ28" s="9"/>
+      <c r="BK28" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BL28" s="3"/>
-      <c r="BM28" s="3"/>
-      <c r="BN28" s="3"/>
-      <c r="BO28" s="3"/>
-      <c r="BP28" s="3"/>
-      <c r="BQ28" s="3"/>
-      <c r="BR28" s="3"/>
-      <c r="BS28" s="3"/>
-      <c r="BT28" s="3"/>
-      <c r="BU28" s="3" t="s">
+      <c r="BL28" s="9"/>
+      <c r="BM28" s="9"/>
+      <c r="BN28" s="9"/>
+      <c r="BO28" s="9"/>
+      <c r="BP28" s="9"/>
+      <c r="BQ28" s="9"/>
+      <c r="BR28" s="9"/>
+      <c r="BS28" s="9"/>
+      <c r="BT28" s="9"/>
+      <c r="BU28" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BV28" s="3"/>
-      <c r="BW28" s="3"/>
-      <c r="BX28" s="3"/>
-      <c r="BY28" s="3"/>
-      <c r="BZ28" s="3"/>
-      <c r="CA28" s="3"/>
-      <c r="CB28" s="3"/>
-      <c r="CC28" s="3"/>
-      <c r="CD28" s="3"/>
-      <c r="CE28" s="3"/>
-      <c r="CF28" s="3"/>
+      <c r="BV28" s="9"/>
+      <c r="BW28" s="9"/>
+      <c r="BX28" s="9"/>
+      <c r="BY28" s="9"/>
+      <c r="BZ28" s="9"/>
+      <c r="CA28" s="9"/>
+      <c r="CB28" s="9"/>
+      <c r="CC28" s="9"/>
+      <c r="CD28" s="9"/>
+      <c r="CE28" s="9"/>
+      <c r="CF28" s="9"/>
     </row>
     <row r="29" spans="1:84" ht="16.5">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="3"/>
-      <c r="AG29" s="3"/>
-      <c r="AH29" s="3"/>
-      <c r="AI29" s="3"/>
-      <c r="AJ29" s="3"/>
-      <c r="AK29" s="3"/>
-      <c r="AL29" s="3"/>
-      <c r="AM29" s="3"/>
-      <c r="AN29" s="3"/>
-      <c r="AO29" s="3"/>
-      <c r="AP29" s="3"/>
-      <c r="AQ29" s="3"/>
-      <c r="AR29" s="3"/>
-      <c r="AS29" s="3"/>
-      <c r="AT29" s="3"/>
-      <c r="AU29" s="3"/>
-      <c r="AV29" s="3"/>
-      <c r="AW29" s="3"/>
-      <c r="AX29" s="3"/>
-      <c r="AY29" s="3"/>
-      <c r="AZ29" s="3"/>
-      <c r="BA29" s="3"/>
-      <c r="BB29" s="3"/>
-      <c r="BC29" s="3"/>
-      <c r="BD29" s="3"/>
-      <c r="BE29" s="3"/>
-      <c r="BF29" s="3"/>
-      <c r="BG29" s="3"/>
-      <c r="BH29" s="3"/>
-      <c r="BI29" s="3"/>
-      <c r="BJ29" s="3"/>
-      <c r="BK29" s="3"/>
-      <c r="BL29" s="3"/>
-      <c r="BM29" s="3"/>
-      <c r="BN29" s="3"/>
-      <c r="BO29" s="3"/>
-      <c r="BP29" s="3"/>
-      <c r="BQ29" s="3"/>
-      <c r="BR29" s="3"/>
-      <c r="BS29" s="3"/>
-      <c r="BT29" s="3"/>
-      <c r="BU29" s="3"/>
-      <c r="BV29" s="3"/>
-      <c r="BW29" s="3"/>
-      <c r="BX29" s="3"/>
-      <c r="BY29" s="3"/>
-      <c r="BZ29" s="3"/>
-      <c r="CA29" s="3"/>
-      <c r="CB29" s="3"/>
-      <c r="CC29" s="3"/>
-      <c r="CD29" s="3"/>
-      <c r="CE29" s="3"/>
-      <c r="CF29" s="3"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V29" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="5"/>
+      <c r="AW29" s="5"/>
+      <c r="AX29" s="5"/>
+      <c r="AY29" s="5"/>
+      <c r="AZ29" s="5"/>
+      <c r="BA29" s="5"/>
+      <c r="BB29" s="5"/>
+      <c r="BC29" s="5"/>
+      <c r="BD29" s="5"/>
+      <c r="BE29" s="5"/>
+      <c r="BF29" s="5"/>
+      <c r="BG29" s="5"/>
+      <c r="BH29" s="5"/>
+      <c r="BI29" s="5"/>
+      <c r="BJ29" s="5"/>
+      <c r="BK29" s="5"/>
+      <c r="BL29" s="5"/>
+      <c r="BM29" s="5"/>
+      <c r="BN29" s="5"/>
+      <c r="BO29" s="5"/>
+      <c r="BP29" s="5"/>
+      <c r="BQ29" s="5"/>
+      <c r="BR29" s="5"/>
+      <c r="BS29" s="5"/>
+      <c r="BT29" s="5"/>
+      <c r="BU29" s="5"/>
+      <c r="BV29" s="5"/>
+      <c r="BW29" s="5"/>
+      <c r="BX29" s="5"/>
+      <c r="BY29" s="5"/>
+      <c r="BZ29" s="5"/>
+      <c r="CA29" s="5"/>
+      <c r="CB29" s="5"/>
+      <c r="CC29" s="5"/>
+      <c r="CD29" s="2"/>
+      <c r="CE29" s="9"/>
+      <c r="CF29" s="9"/>
     </row>
     <row r="30" spans="1:84" ht="16.5">
-      <c r="E30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="10" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N30" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="O30" s="3"/>
-      <c r="P30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q30" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S30" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="T30" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="V30" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W30" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ30" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP30" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ30" s="6"/>
-      <c r="AR30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AS30" s="6"/>
-      <c r="AT30" s="6"/>
-      <c r="AU30" s="6"/>
-      <c r="AV30" s="6"/>
-      <c r="AW30" s="6"/>
-      <c r="AX30" s="6"/>
-      <c r="AY30" s="6"/>
-      <c r="AZ30" s="6"/>
-      <c r="BA30" s="6"/>
-      <c r="BB30" s="6"/>
-      <c r="BC30" s="6"/>
-      <c r="BD30" s="6"/>
-      <c r="BE30" s="6"/>
-      <c r="BF30" s="6"/>
-      <c r="BG30" s="6"/>
-      <c r="BH30" s="6"/>
-      <c r="BI30" s="6"/>
-      <c r="BJ30" s="6"/>
-      <c r="BK30" s="6"/>
-      <c r="BL30" s="6"/>
-      <c r="BM30" s="6"/>
-      <c r="BN30" s="6"/>
-      <c r="BO30" s="6"/>
-      <c r="BP30" s="6"/>
-      <c r="BQ30" s="6"/>
-      <c r="BR30" s="6"/>
-      <c r="BS30" s="6"/>
-      <c r="BT30" s="6"/>
-      <c r="BU30" s="6"/>
-      <c r="BV30" s="6"/>
-      <c r="BW30" s="6"/>
-      <c r="BX30" s="6"/>
-      <c r="BY30" s="6"/>
-      <c r="BZ30" s="6"/>
-      <c r="CA30" s="6"/>
-      <c r="CB30" s="6"/>
-      <c r="CC30" s="6"/>
-      <c r="CD30" s="2"/>
-      <c r="CE30" s="1" t="s">
+      <c r="R30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="V30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="X30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="CF30" s="1" t="s">
+      <c r="AB30" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="AC30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AX30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BI30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BL30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BM30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BN30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="BP30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BS30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="BU30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BV30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BW30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BX30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="BZ30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="CB30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="CD30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="CE30" s="9"/>
+      <c r="CF30" s="9"/>
     </row>
     <row r="31" spans="1:84" ht="16.5">
-      <c r="P31" s="3" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R31" s="3" t="s">
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="9"/>
+      <c r="AL31" s="9"/>
+      <c r="AM31" s="9"/>
+      <c r="AN31" s="9"/>
+      <c r="AO31" s="9"/>
+      <c r="AP31" s="9"/>
+      <c r="AQ31" s="9"/>
+      <c r="AR31" s="9"/>
+      <c r="AS31" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="AT31" s="9"/>
+      <c r="AU31" s="9"/>
+      <c r="AV31" s="9"/>
+      <c r="AW31" s="9"/>
+      <c r="AX31" s="9"/>
+      <c r="AY31" s="9"/>
+      <c r="AZ31" s="9"/>
+      <c r="BA31" s="9"/>
+      <c r="BB31" s="9"/>
+      <c r="BC31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="T31" s="3" t="s">
+      <c r="BD31" s="9"/>
+      <c r="BE31" s="9"/>
+      <c r="BF31" s="9"/>
+      <c r="BG31" s="9"/>
+      <c r="BH31" s="9"/>
+      <c r="BI31" s="9"/>
+      <c r="BJ31" s="9"/>
+      <c r="BK31" s="9"/>
+      <c r="BL31" s="9"/>
+      <c r="BM31" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="U31" s="3" t="s">
+      <c r="BN31" s="9"/>
+      <c r="BO31" s="9"/>
+      <c r="BP31" s="9"/>
+      <c r="BQ31" s="9"/>
+      <c r="BR31" s="9"/>
+      <c r="BS31" s="9"/>
+      <c r="BT31" s="9"/>
+      <c r="BU31" s="9"/>
+      <c r="BV31" s="9"/>
+      <c r="BW31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="W31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="X31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AN31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AR31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AT31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AU31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AW31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="BA31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="BB31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BC31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="BD31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="BF31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="BG31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BH31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="BI31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="BJ31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="BK31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="BL31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BM31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="BN31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="BO31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="BP31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="BQ31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BR31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="BS31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="BT31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="BU31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="BV31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BW31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="BX31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="BY31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="BZ31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="CA31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="CB31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="CC31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="CD31" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:84" ht="16.5">
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z32" s="3"/>
-      <c r="AA32" s="3"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="3"/>
-      <c r="AE32" s="3"/>
-      <c r="AF32" s="3"/>
-      <c r="AG32" s="3"/>
-      <c r="AH32" s="3"/>
-      <c r="AI32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ32" s="3"/>
-      <c r="AK32" s="3"/>
-      <c r="AL32" s="3"/>
-      <c r="AM32" s="3"/>
-      <c r="AN32" s="3"/>
-      <c r="AO32" s="3"/>
-      <c r="AP32" s="3"/>
-      <c r="AQ32" s="3"/>
-      <c r="AR32" s="3"/>
-      <c r="AS32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT32" s="3"/>
-      <c r="AU32" s="3"/>
-      <c r="AV32" s="3"/>
-      <c r="AW32" s="3"/>
-      <c r="AX32" s="3"/>
-      <c r="AY32" s="3"/>
-      <c r="AZ32" s="3"/>
-      <c r="BA32" s="3"/>
-      <c r="BB32" s="3"/>
-      <c r="BC32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BD32" s="3"/>
-      <c r="BE32" s="3"/>
-      <c r="BF32" s="3"/>
-      <c r="BG32" s="3"/>
-      <c r="BH32" s="3"/>
-      <c r="BI32" s="3"/>
-      <c r="BJ32" s="3"/>
-      <c r="BK32" s="3"/>
-      <c r="BL32" s="3"/>
-      <c r="BM32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="BN32" s="3"/>
-      <c r="BO32" s="3"/>
-      <c r="BP32" s="3"/>
-      <c r="BQ32" s="3"/>
-      <c r="BR32" s="3"/>
-      <c r="BS32" s="3"/>
-      <c r="BT32" s="3"/>
-      <c r="BU32" s="3"/>
-      <c r="BV32" s="3"/>
-      <c r="BW32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="BX32" s="3"/>
-      <c r="BY32" s="3"/>
-      <c r="BZ32" s="3"/>
-      <c r="CA32" s="3"/>
-      <c r="CB32" s="3"/>
-      <c r="CC32" s="3"/>
-      <c r="CD32" s="3"/>
+      <c r="BX31" s="9"/>
+      <c r="BY31" s="9"/>
+      <c r="BZ31" s="9"/>
+      <c r="CA31" s="9"/>
+      <c r="CB31" s="9"/>
+      <c r="CC31" s="9"/>
+      <c r="CD31" s="9"/>
+      <c r="CE31" s="9"/>
+      <c r="CF31" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>